<commit_message>
Auto Edge driver update
</commit_message>
<xml_diff>
--- a/Scraping/Linkage Disequilibrium/output/output_toscani.xlsx
+++ b/Scraping/Linkage Disequilibrium/output/output_toscani.xlsx
@@ -509,10 +509,8 @@
           <t>rs72916782</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1.000000</t>
-        </is>
+      <c r="B3" t="n">
+        <v>-1</v>
       </c>
       <c r="C3" t="n">
         <v>-1</v>
@@ -539,10 +537,8 @@
           <t>rs72916784</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0.761244</t>
-        </is>
+      <c r="B4" t="n">
+        <v>-1</v>
       </c>
       <c r="C4" t="n">
         <v>-1</v>

</xml_diff>